<commit_message>
fix std cant A45 problem
</commit_message>
<xml_diff>
--- a/NotchMappingTable.xlsx
+++ b/NotchMappingTable.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\Git\DENSYAGO_OHCPC01A_TO_NS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F651E4-F1F4-4FFE-979E-91BC20131A19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="28035" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>EB</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -109,55 +115,6 @@
   </si>
   <si>
     <t>-70</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>-100</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>90-&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="3" tint="0.39997558519241921"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -100</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">70 -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>80</t>
-    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -217,12 +174,55 @@
     <t>103 系</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">70 -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>80</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,24 +248,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="新細明體"/>
       <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="3" tint="0.39997558519241921"/>
-      <name val="新細明體"/>
-      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -278,20 +262,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4"/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Yu Gothic"/>
       <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -490,7 +480,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -521,16 +511,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -569,13 +556,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -587,6 +574,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -633,7 +628,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,9 +660,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -699,6 +712,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -874,22 +905,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="9" customWidth="1"/>
     <col min="10" max="10" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="17.25" thickBot="1"/>
-    <row r="2" spans="2:10">
-      <c r="B2" s="24"/>
+    <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
@@ -897,43 +928,43 @@
         <v>205</v>
       </c>
       <c r="E2" s="27"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="24"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="29"/>
+        <v>33</v>
+      </c>
+      <c r="I2" s="28"/>
       <c r="J2" s="27"/>
     </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="18" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="18" t="s">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -943,11 +974,11 @@
       <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="9"/>
@@ -955,45 +986,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>-100</v>
+        <v>-90</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="5">
-        <v>100</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>-90</v>
+        <v>-80</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5">
-        <v>90</v>
-      </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="9"/>
@@ -1001,22 +1032,22 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="18" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>-80</v>
+        <v>-75</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5">
-        <v>80</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="9"/>
@@ -1024,8 +1055,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="18" t="s">
+    <row r="8" spans="2:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2">
@@ -1035,20 +1066,20 @@
       <c r="E8" s="5">
         <v>70</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="21"/>
+      <c r="G8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>29</v>
+      <c r="H8" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2">
@@ -1058,11 +1089,11 @@
       <c r="E9" s="5">
         <v>60</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="18" t="s">
+      <c r="F9" s="21"/>
+      <c r="G9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="9"/>
@@ -1070,8 +1101,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="18" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2">
@@ -1081,11 +1112,11 @@
       <c r="E10" s="5">
         <v>50</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="18" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="9"/>
@@ -1093,8 +1124,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="18" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2">
@@ -1104,11 +1135,11 @@
       <c r="E11" s="5">
         <v>40</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="18" t="s">
+      <c r="F11" s="21"/>
+      <c r="G11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="9"/>
@@ -1116,8 +1147,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="18" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="2">
@@ -1127,11 +1158,11 @@
       <c r="E12" s="5">
         <v>30</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="18" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I12" s="9"/>
@@ -1139,33 +1170,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="20" t="s">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>0</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <v>0</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>0</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="16">
+      <c r="H13" s="19"/>
+      <c r="I13" s="15">
         <v>0</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="18" t="s">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="2">
@@ -1175,11 +1206,11 @@
         <v>30</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="18" t="s">
+      <c r="F14" s="22"/>
+      <c r="G14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>10</v>
       </c>
       <c r="I14" s="12" t="s">
@@ -1187,8 +1218,8 @@
       </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="18" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="2">
@@ -1198,11 +1229,11 @@
         <v>50</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="18" t="s">
+      <c r="F15" s="22"/>
+      <c r="G15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="12" t="s">
@@ -1210,8 +1241,8 @@
       </c>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="18" t="s">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2">
@@ -1221,11 +1252,11 @@
         <v>70</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="18" t="s">
+      <c r="F16" s="22"/>
+      <c r="G16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I16" s="12" t="s">
@@ -1233,49 +1264,49 @@
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="18" t="s">
+    <row r="17" spans="2:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="2">
+        <v>80</v>
+      </c>
+      <c r="D17" s="4">
+        <v>80</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3">
         <v>90</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D18" s="7">
         <v>90</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="2:10" ht="17.25" thickBot="1">
-      <c r="B18" s="21" t="s">
+      <c r="E18" s="8"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3">
-        <v>100</v>
-      </c>
-      <c r="D18" s="7">
-        <v>100</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>26</v>
+      <c r="I18" s="13">
+        <v>-90</v>
       </c>
       <c r="J18" s="8"/>
     </row>
@@ -1286,17 +1317,17 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1304,12 +1335,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed the value to max 100, and tested in game E231, 103, 205
</commit_message>
<xml_diff>
--- a/NotchMappingTable.xlsx
+++ b/NotchMappingTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\Git\DENSYAGO_OHCPC01A_TO_NS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F651E4-F1F4-4FFE-979E-91BC20131A19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B50F80-7694-4BAE-9078-719FC68FE227}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,14 +22,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>EB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>B8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>B7</t>
@@ -54,15 +54,15 @@
   </si>
   <si>
     <t>N</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>P1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>P2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>P3</t>
@@ -75,165 +75,80 @@
   </si>
   <si>
     <t>E231</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>L2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>B4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>B3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>B2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>B1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>P3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>P4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>-30</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>-50</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>-70</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>B2 -&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> B3</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">P3 -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P4</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Notch</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>103 Notch</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LX</t>
   </si>
   <si>
     <t>RX</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>103 系</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">70 -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>80</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -254,34 +169,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="4"/>
-      <name val="Yu Gothic"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Yu Gothic"/>
-      <family val="2"/>
-      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -480,7 +373,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -511,10 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -533,9 +423,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -556,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -909,7 +796,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -920,51 +807,51 @@
   <sheetData>
     <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="24">
         <v>205</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="27"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="26"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="25" t="s">
+      <c r="J3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -974,11 +861,11 @@
       <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="9"/>
@@ -987,53 +874,53 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>-90</v>
+        <v>-100</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="5">
-        <v>90</v>
-      </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="10">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>-80</v>
+        <v>-85</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5">
-        <v>80</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="10">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2">
@@ -1043,11 +930,11 @@
       <c r="E7" s="5">
         <v>75</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="19"/>
+      <c r="G7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="9"/>
@@ -1055,8 +942,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2">
@@ -1066,20 +953,20 @@
       <c r="E8" s="5">
         <v>70</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="17" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>26</v>
+      <c r="H8" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="11" t="s">
-        <v>34</v>
+      <c r="J8" s="5">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2">
@@ -1089,11 +976,11 @@
       <c r="E9" s="5">
         <v>60</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="17" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="9"/>
@@ -1102,7 +989,7 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2">
@@ -1112,11 +999,11 @@
       <c r="E10" s="5">
         <v>50</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="17" t="s">
+      <c r="F10" s="19"/>
+      <c r="G10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="9"/>
@@ -1125,7 +1012,7 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2">
@@ -1135,11 +1022,11 @@
       <c r="E11" s="5">
         <v>40</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="17" t="s">
+      <c r="F11" s="19"/>
+      <c r="G11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="9"/>
@@ -1148,7 +1035,7 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="2">
@@ -1158,11 +1045,11 @@
       <c r="E12" s="5">
         <v>30</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="17" t="s">
+      <c r="F12" s="19"/>
+      <c r="G12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>20</v>
       </c>
       <c r="I12" s="9"/>
@@ -1171,32 +1058,32 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>0</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>0</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="15">
         <v>0</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="15">
+      <c r="H13" s="17"/>
+      <c r="I13" s="14">
         <v>0</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="2">
@@ -1206,20 +1093,20 @@
         <v>30</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="17" t="s">
+      <c r="F14" s="20"/>
+      <c r="G14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="2">
@@ -1229,20 +1116,20 @@
         <v>50</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="17" t="s">
+      <c r="F15" s="20"/>
+      <c r="G15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2">
@@ -1252,61 +1139,61 @@
         <v>70</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="17" t="s">
+      <c r="F16" s="20"/>
+      <c r="G16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>25</v>
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:10" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
+    <row r="17" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="2">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D17" s="4">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="17" t="s">
+      <c r="F17" s="20"/>
+      <c r="G17" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="I17" s="11">
+        <v>-100</v>
       </c>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="3">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D18" s="7">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="20" t="s">
+      <c r="F18" s="20"/>
+      <c r="G18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="13">
-        <v>-90</v>
+      <c r="I18" s="12">
+        <v>-100</v>
       </c>
       <c r="J18" s="8"/>
     </row>
@@ -1315,7 +1202,7 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="H2:J2"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -1329,7 +1216,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1342,7 +1229,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>